<commit_message>
Still needs a way to msmethod to Preblank in a two column system. Attempt with TB_method variable was unsucessful.
</commit_message>
<xml_diff>
--- a/JM1013_worklist_50_Cond_Format.xlsx
+++ b/JM1013_worklist_50_Cond_Format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01c1829094dbd390/Desktop/Kelly_Lab/.venv/worklist_git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivint\OneDrive\Desktop\Kelly_Lab\.venv\worklist_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{11B0C519-5E91-4115-8B3E-F954851F6711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48B0916D-6A2F-4E40-B1FE-891DB7BA5532}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE238A2-7FF0-4A38-8DF4-507B06B3908E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{12DA0CF9-A1F3-4B47-B73A-18ED55D7EBC7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="80">
   <si>
     <t>Notebook code:</t>
   </si>
@@ -194,12 +194,6 @@
     <t>mypath</t>
   </si>
   <si>
-    <t>2 column</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
     <t xml:space="preserve">UofU LCM Samples Plate 1 </t>
   </si>
   <si>
@@ -209,24 +203,12 @@
     <t>Slide 39 TMEV CA1</t>
   </si>
   <si>
-    <t>msdatapath</t>
-  </si>
-  <si>
-    <t>msmethodpath</t>
-  </si>
-  <si>
     <t>dry</t>
   </si>
   <si>
     <t>LF_12ms</t>
   </si>
   <si>
-    <t>lcdatapath</t>
-  </si>
-  <si>
-    <t>lcmethodpath</t>
-  </si>
-  <si>
     <t>wet</t>
   </si>
   <si>
@@ -278,23 +260,32 @@
     <t>Before</t>
   </si>
   <si>
-    <t>TrueBlank</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>1-12</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>1 column</t>
+  </si>
+  <si>
+    <t>D:\Data\Tyler.H\JM1013</t>
+  </si>
+  <si>
+    <t>C:\Data\Tyler\Methods\RightColumn_200nldry</t>
+  </si>
+  <si>
+    <t>C:\Data\Tyler\Methods\ChannelA_flush_1min_1ul</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,6 +305,16 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="-Apple-System"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -509,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -570,45 +571,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -637,6 +599,47 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,10 +655,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -978,10 +977,10 @@
   <dimension ref="A1:AV63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="42" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="AL43" sqref="AL43"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
@@ -1004,7 +1003,7 @@
     <col min="43" max="45" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:48">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1059,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:48">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1070,101 +1069,101 @@
       <c r="AD2" s="12">
         <v>1</v>
       </c>
-      <c r="AE2" s="46" t="s">
+      <c r="AE2" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF2" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH2" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI2" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF2" s="47" t="s">
+      <c r="AJ2" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AG2" s="48" t="s">
+      <c r="AK2" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM2" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="28" t="s">
+      <c r="AN2" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI2" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ2" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK2" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL2" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM2" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN2" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO2" s="28">
         <v>1</v>
       </c>
       <c r="AP2" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ2" s="12"/>
       <c r="AR2" s="12"/>
       <c r="AS2" s="11"/>
     </row>
-    <row r="3" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:48" ht="16" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="AD3" s="12">
         <v>2</v>
       </c>
       <c r="AE3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH3" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI3" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG3" s="48" t="s">
+      <c r="AJ3" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL3" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM3" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH3" s="28" t="s">
+      <c r="AN3" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI3" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ3" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK3" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL3" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM3" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN3" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO3" s="29">
         <v>1</v>
       </c>
       <c r="AP3" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ3" s="12"/>
       <c r="AR3" s="12"/>
       <c r="AS3" s="11"/>
-      <c r="AU3" s="30" t="s">
+      <c r="AU3" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="AV3" s="30"/>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AV3" s="50"/>
+    </row>
+    <row r="4" spans="1:48">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="D4" s="3"/>
@@ -1196,48 +1195,48 @@
         <v>3</v>
       </c>
       <c r="AE4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF4" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG4" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH4" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI4" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF4" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG4" s="48" t="s">
+      <c r="AJ4" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK4" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL4" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM4" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH4" s="28" t="s">
+      <c r="AN4" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI4" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ4" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK4" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL4" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM4" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN4" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO4" s="29">
         <v>1</v>
       </c>
       <c r="AP4" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ4" s="12"/>
       <c r="AR4" s="12"/>
       <c r="AS4" s="11"/>
-      <c r="AU4" s="30"/>
-      <c r="AV4" s="30"/>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU4" s="50"/>
+      <c r="AV4" s="50"/>
+    </row>
+    <row r="5" spans="1:48">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1323,53 +1322,53 @@
         <v>4</v>
       </c>
       <c r="AE5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG5" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH5" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI5" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG5" s="48" t="s">
+      <c r="AJ5" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK5" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL5" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM5" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH5" s="28" t="s">
+      <c r="AN5" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI5" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ5" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK5" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL5" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM5" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN5" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO5" s="29">
         <v>1</v>
       </c>
       <c r="AP5" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ5" s="12"/>
       <c r="AR5" s="12"/>
       <c r="AS5" s="11"/>
-      <c r="AU5" s="30"/>
-      <c r="AV5" s="30"/>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU5" s="50"/>
+      <c r="AV5" s="50"/>
+    </row>
+    <row r="6" spans="1:48">
       <c r="A6" s="13" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -1402,48 +1401,48 @@
         <v>5</v>
       </c>
       <c r="AE6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF6" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG6" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH6" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI6" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF6" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG6" s="48" t="s">
+      <c r="AJ6" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK6" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL6" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM6" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH6" s="28" t="s">
+      <c r="AN6" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI6" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ6" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK6" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL6" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM6" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN6" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO6" s="28">
         <v>1</v>
       </c>
       <c r="AP6" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ6" s="12"/>
       <c r="AR6" s="12"/>
       <c r="AS6" s="11"/>
-      <c r="AU6" s="30"/>
-      <c r="AV6" s="30"/>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU6" s="50"/>
+      <c r="AV6" s="50"/>
+    </row>
+    <row r="7" spans="1:48">
       <c r="D7" t="s">
         <v>18</v>
       </c>
@@ -1475,100 +1474,100 @@
         <v>6</v>
       </c>
       <c r="AE7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG7" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH7" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI7" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG7" s="48" t="s">
+      <c r="AJ7" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK7" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL7" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM7" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH7" s="28" t="s">
+      <c r="AN7" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI7" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ7" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK7" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL7" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM7" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN7" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO7" s="29">
         <v>1</v>
       </c>
       <c r="AP7" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ7" s="12"/>
       <c r="AR7" s="12"/>
       <c r="AS7" s="11"/>
-      <c r="AU7" s="30"/>
-      <c r="AV7" s="30"/>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU7" s="50"/>
+      <c r="AV7" s="50"/>
+    </row>
+    <row r="8" spans="1:48">
       <c r="D8" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="43">
+      <c r="F8" s="30">
         <v>1</v>
       </c>
       <c r="G8" s="10">
         <v>2</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="30">
         <v>3</v>
       </c>
       <c r="I8" s="10">
         <v>4</v>
       </c>
-      <c r="J8" s="43">
+      <c r="J8" s="30">
         <v>5</v>
       </c>
       <c r="K8" s="10">
         <v>6</v>
       </c>
-      <c r="L8" s="43">
+      <c r="L8" s="30">
         <v>7</v>
       </c>
       <c r="M8" s="10">
         <v>8</v>
       </c>
-      <c r="N8" s="43">
+      <c r="N8" s="30">
         <v>9</v>
       </c>
       <c r="O8" s="10">
         <v>10</v>
       </c>
       <c r="P8" s="10"/>
-      <c r="Q8" s="44">
+      <c r="Q8" s="31">
         <v>11</v>
       </c>
-      <c r="R8" s="44">
+      <c r="R8" s="31">
         <v>11</v>
       </c>
-      <c r="S8" s="44">
+      <c r="S8" s="31">
         <v>11</v>
       </c>
       <c r="T8" s="10"/>
-      <c r="U8" s="45">
+      <c r="U8" s="32">
         <v>12</v>
       </c>
-      <c r="V8" s="45">
+      <c r="V8" s="32">
         <v>12</v>
       </c>
-      <c r="W8" s="45">
+      <c r="W8" s="32">
         <v>12</v>
       </c>
       <c r="X8" s="10"/>
@@ -1580,100 +1579,100 @@
         <v>7</v>
       </c>
       <c r="AE8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF8" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG8" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH8" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI8" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF8" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG8" s="48" t="s">
+      <c r="AJ8" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK8" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL8" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM8" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH8" s="28" t="s">
+      <c r="AN8" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI8" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ8" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK8" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL8" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM8" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN8" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO8" s="29">
         <v>1</v>
       </c>
       <c r="AP8" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ8" s="12"/>
       <c r="AR8" s="12"/>
       <c r="AS8" s="11"/>
-      <c r="AU8" s="30"/>
-      <c r="AV8" s="30"/>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU8" s="50"/>
+      <c r="AV8" s="50"/>
+    </row>
+    <row r="9" spans="1:48">
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="43">
+      <c r="F9" s="30">
         <v>1</v>
       </c>
       <c r="G9" s="10">
         <v>2</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="30">
         <v>3</v>
       </c>
       <c r="I9" s="10">
         <v>4</v>
       </c>
-      <c r="J9" s="43">
+      <c r="J9" s="30">
         <v>5</v>
       </c>
       <c r="K9" s="10">
         <v>6</v>
       </c>
-      <c r="L9" s="43">
+      <c r="L9" s="30">
         <v>7</v>
       </c>
       <c r="M9" s="10">
         <v>8</v>
       </c>
-      <c r="N9" s="43">
+      <c r="N9" s="30">
         <v>9</v>
       </c>
       <c r="O9" s="10">
         <v>10</v>
       </c>
       <c r="P9" s="10"/>
-      <c r="Q9" s="44">
+      <c r="Q9" s="31">
         <v>11</v>
       </c>
-      <c r="R9" s="44">
+      <c r="R9" s="31">
         <v>11</v>
       </c>
-      <c r="S9" s="44">
+      <c r="S9" s="31">
         <v>11</v>
       </c>
       <c r="T9" s="10"/>
-      <c r="U9" s="45">
+      <c r="U9" s="32">
         <v>12</v>
       </c>
-      <c r="V9" s="45">
+      <c r="V9" s="32">
         <v>12</v>
       </c>
-      <c r="W9" s="45">
+      <c r="W9" s="32">
         <v>12</v>
       </c>
       <c r="X9" s="10"/>
@@ -1685,100 +1684,100 @@
         <v>8</v>
       </c>
       <c r="AE9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG9" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH9" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI9" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF9" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG9" s="48" t="s">
+      <c r="AJ9" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK9" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL9" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM9" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH9" s="28" t="s">
+      <c r="AN9" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI9" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ9" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK9" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL9" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM9" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN9" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO9" s="29">
         <v>1</v>
       </c>
       <c r="AP9" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ9" s="12"/>
       <c r="AR9" s="12"/>
       <c r="AS9" s="11"/>
-      <c r="AU9" s="30"/>
-      <c r="AV9" s="30"/>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU9" s="50"/>
+      <c r="AV9" s="50"/>
+    </row>
+    <row r="10" spans="1:48">
       <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="43">
+      <c r="F10" s="30">
         <v>1</v>
       </c>
       <c r="G10" s="10">
         <v>2</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="30">
         <v>3</v>
       </c>
       <c r="I10" s="10">
         <v>4</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="30">
         <v>5</v>
       </c>
       <c r="K10" s="10">
         <v>6</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L10" s="30">
         <v>7</v>
       </c>
       <c r="M10" s="10">
         <v>8</v>
       </c>
-      <c r="N10" s="43">
+      <c r="N10" s="30">
         <v>9</v>
       </c>
       <c r="O10" s="10">
         <v>10</v>
       </c>
       <c r="P10" s="10"/>
-      <c r="Q10" s="44">
+      <c r="Q10" s="31">
         <v>11</v>
       </c>
-      <c r="R10" s="44">
+      <c r="R10" s="31">
         <v>11</v>
       </c>
-      <c r="S10" s="44">
+      <c r="S10" s="31">
         <v>11</v>
       </c>
       <c r="T10" s="10"/>
-      <c r="U10" s="45">
+      <c r="U10" s="32">
         <v>12</v>
       </c>
-      <c r="V10" s="45">
+      <c r="V10" s="32">
         <v>12</v>
       </c>
-      <c r="W10" s="45">
+      <c r="W10" s="32">
         <v>12</v>
       </c>
       <c r="X10" s="10"/>
@@ -1790,100 +1789,100 @@
         <v>9</v>
       </c>
       <c r="AE10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF10" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG10" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH10" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI10" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF10" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG10" s="48" t="s">
+      <c r="AJ10" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK10" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL10" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM10" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH10" s="28" t="s">
+      <c r="AN10" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI10" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ10" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK10" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL10" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM10" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN10" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO10" s="28">
         <v>1</v>
       </c>
       <c r="AP10" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ10" s="12"/>
       <c r="AR10" s="12"/>
       <c r="AS10" s="11"/>
-      <c r="AU10" s="30"/>
-      <c r="AV10" s="30"/>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU10" s="50"/>
+      <c r="AV10" s="50"/>
+    </row>
+    <row r="11" spans="1:48">
       <c r="D11" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="43">
+      <c r="F11" s="30">
         <v>1</v>
       </c>
       <c r="G11" s="10">
         <v>2</v>
       </c>
-      <c r="H11" s="43">
+      <c r="H11" s="30">
         <v>3</v>
       </c>
       <c r="I11" s="10">
         <v>4</v>
       </c>
-      <c r="J11" s="43">
+      <c r="J11" s="30">
         <v>5</v>
       </c>
       <c r="K11" s="10">
         <v>6</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="30">
         <v>7</v>
       </c>
       <c r="M11" s="10">
         <v>8</v>
       </c>
-      <c r="N11" s="43">
+      <c r="N11" s="30">
         <v>9</v>
       </c>
       <c r="O11" s="10">
         <v>10</v>
       </c>
       <c r="P11" s="10"/>
-      <c r="Q11" s="44">
+      <c r="Q11" s="31">
         <v>11</v>
       </c>
-      <c r="R11" s="44">
+      <c r="R11" s="31">
         <v>11</v>
       </c>
-      <c r="S11" s="44">
+      <c r="S11" s="31">
         <v>11</v>
       </c>
       <c r="T11" s="10"/>
-      <c r="U11" s="45">
+      <c r="U11" s="32">
         <v>12</v>
       </c>
-      <c r="V11" s="45">
+      <c r="V11" s="32">
         <v>12</v>
       </c>
-      <c r="W11" s="45">
+      <c r="W11" s="32">
         <v>12</v>
       </c>
       <c r="X11" s="10"/>
@@ -1895,100 +1894,100 @@
         <v>10</v>
       </c>
       <c r="AE11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG11" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH11" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI11" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AF11" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG11" s="48" t="s">
+      <c r="AJ11" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK11" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL11" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM11" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH11" s="28" t="s">
+      <c r="AN11" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI11" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ11" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK11" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL11" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM11" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN11" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO11" s="29">
         <v>1</v>
       </c>
       <c r="AP11" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ11" s="12"/>
       <c r="AR11" s="12"/>
       <c r="AS11" s="11"/>
-      <c r="AU11" s="30"/>
-      <c r="AV11" s="30"/>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU11" s="50"/>
+      <c r="AV11" s="50"/>
+    </row>
+    <row r="12" spans="1:48">
       <c r="D12" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="43">
+      <c r="F12" s="30">
         <v>1</v>
       </c>
       <c r="G12" s="10">
         <v>2</v>
       </c>
-      <c r="H12" s="43">
+      <c r="H12" s="30">
         <v>3</v>
       </c>
       <c r="I12" s="10">
         <v>4</v>
       </c>
-      <c r="J12" s="43">
+      <c r="J12" s="30">
         <v>5</v>
       </c>
       <c r="K12" s="10">
         <v>6</v>
       </c>
-      <c r="L12" s="43">
+      <c r="L12" s="30">
         <v>7</v>
       </c>
       <c r="M12" s="10">
         <v>8</v>
       </c>
-      <c r="N12" s="43">
+      <c r="N12" s="30">
         <v>9</v>
       </c>
       <c r="O12" s="10">
         <v>10</v>
       </c>
       <c r="P12" s="10"/>
-      <c r="Q12" s="44">
+      <c r="Q12" s="31">
         <v>11</v>
       </c>
-      <c r="R12" s="44">
+      <c r="R12" s="31">
         <v>11</v>
       </c>
-      <c r="S12" s="44">
+      <c r="S12" s="31">
         <v>11</v>
       </c>
       <c r="T12" s="10"/>
-      <c r="U12" s="45">
+      <c r="U12" s="32">
         <v>12</v>
       </c>
-      <c r="V12" s="45">
+      <c r="V12" s="32">
         <v>12</v>
       </c>
-      <c r="W12" s="45">
+      <c r="W12" s="32">
         <v>12</v>
       </c>
       <c r="X12" s="10"/>
@@ -2000,40 +1999,40 @@
         <v>11</v>
       </c>
       <c r="AE12" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF12" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG12" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF12" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG12" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH12" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI12" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ12" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK12" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL12" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM12" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH12" s="28" t="s">
+      <c r="AN12" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI12" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ12" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK12" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL12" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM12" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN12" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO12" s="29">
         <v>1</v>
       </c>
       <c r="AP12" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ12" s="12">
         <v>3</v>
@@ -2044,10 +2043,10 @@
       <c r="AS12" s="11">
         <v>12</v>
       </c>
-      <c r="AU12" s="30"/>
-      <c r="AV12" s="30"/>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU12" s="50"/>
+      <c r="AV12" s="50"/>
+    </row>
+    <row r="13" spans="1:48">
       <c r="D13" t="s">
         <v>24</v>
       </c>
@@ -2063,23 +2062,23 @@
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
-      <c r="Q13" s="44">
+      <c r="Q13" s="31">
         <v>11</v>
       </c>
-      <c r="R13" s="44">
+      <c r="R13" s="31">
         <v>11</v>
       </c>
-      <c r="S13" s="44">
+      <c r="S13" s="31">
         <v>11</v>
       </c>
       <c r="T13" s="10"/>
-      <c r="U13" s="45">
+      <c r="U13" s="32">
         <v>12</v>
       </c>
-      <c r="V13" s="45">
+      <c r="V13" s="32">
         <v>12</v>
       </c>
-      <c r="W13" s="45">
+      <c r="W13" s="32">
         <v>12</v>
       </c>
       <c r="X13" s="10"/>
@@ -2091,40 +2090,40 @@
         <v>12</v>
       </c>
       <c r="AE13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF13" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG13" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="AF13" s="54" t="s">
+      <c r="AH13" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="AG13" s="48" t="s">
+      <c r="AI13" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ13" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK13" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL13" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM13" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="AH13" s="28" t="s">
+      <c r="AN13" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="AI13" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ13" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK13" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL13" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM13" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN13" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="AO13" s="29">
         <v>1</v>
       </c>
       <c r="AP13" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AQ13" s="12">
         <v>3</v>
@@ -2135,10 +2134,10 @@
       <c r="AS13" s="11">
         <v>12</v>
       </c>
-      <c r="AU13" s="30"/>
-      <c r="AV13" s="30"/>
-    </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU13" s="50"/>
+      <c r="AV13" s="50"/>
+    </row>
+    <row r="14" spans="1:48">
       <c r="D14" t="s">
         <v>25</v>
       </c>
@@ -2184,10 +2183,10 @@
       <c r="AQ14" s="12"/>
       <c r="AR14" s="12"/>
       <c r="AS14" s="11"/>
-      <c r="AU14" s="30"/>
-      <c r="AV14" s="30"/>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.4">
+      <c r="AU14" s="50"/>
+      <c r="AV14" s="50"/>
+    </row>
+    <row r="15" spans="1:48">
       <c r="D15" t="s">
         <v>26</v>
       </c>
@@ -2234,7 +2233,7 @@
       <c r="AR15" s="12"/>
       <c r="AS15" s="11"/>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:48">
       <c r="D16" t="s">
         <v>27</v>
       </c>
@@ -2281,7 +2280,7 @@
       <c r="AR16" s="12"/>
       <c r="AS16" s="11"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:45">
       <c r="D17" t="s">
         <v>28</v>
       </c>
@@ -2328,7 +2327,7 @@
       <c r="AR17" s="12"/>
       <c r="AS17" s="11"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:45">
       <c r="D18" t="s">
         <v>29</v>
       </c>
@@ -2375,7 +2374,7 @@
       <c r="AR18" s="12"/>
       <c r="AS18" s="11"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:45">
       <c r="D19" t="s">
         <v>30</v>
       </c>
@@ -2422,14 +2421,12 @@
       <c r="AR19" s="12"/>
       <c r="AS19" s="11"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:45">
       <c r="D20" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="10">
-        <v>50</v>
-      </c>
+      <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -2471,7 +2468,7 @@
       <c r="AR20" s="12"/>
       <c r="AS20" s="11"/>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:45">
       <c r="D21" t="s">
         <v>32</v>
       </c>
@@ -2518,7 +2515,7 @@
       <c r="AR21" s="12"/>
       <c r="AS21" s="11"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:45">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
@@ -2565,7 +2562,7 @@
       <c r="AR22" s="12"/>
       <c r="AS22" s="11"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:45">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2663,7 @@
       <c r="AR23" s="12"/>
       <c r="AS23" s="11"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:45">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="D24" t="s">
@@ -2715,7 +2712,7 @@
       <c r="AR24" s="12"/>
       <c r="AS24" s="11"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:45">
       <c r="D25" t="s">
         <v>18</v>
       </c>
@@ -2762,7 +2759,7 @@
       <c r="AR25" s="12"/>
       <c r="AS25" s="11"/>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:45">
       <c r="D26" t="s">
         <v>19</v>
       </c>
@@ -2809,7 +2806,7 @@
       <c r="AR26" s="12"/>
       <c r="AS26" s="11"/>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:45">
       <c r="D27" t="s">
         <v>20</v>
       </c>
@@ -2856,7 +2853,7 @@
       <c r="AR27" s="12"/>
       <c r="AS27" s="11"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:45">
       <c r="D28" t="s">
         <v>21</v>
       </c>
@@ -2903,7 +2900,7 @@
       <c r="AR28" s="12"/>
       <c r="AS28" s="11"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:45">
       <c r="D29" t="s">
         <v>22</v>
       </c>
@@ -2950,7 +2947,7 @@
       <c r="AR29" s="12"/>
       <c r="AS29" s="11"/>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:45">
       <c r="D30" t="s">
         <v>23</v>
       </c>
@@ -2997,7 +2994,7 @@
       <c r="AR30" s="12"/>
       <c r="AS30" s="11"/>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:45">
       <c r="D31" t="s">
         <v>24</v>
       </c>
@@ -3044,7 +3041,7 @@
       <c r="AR31" s="12"/>
       <c r="AS31" s="11"/>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:45">
       <c r="D32" t="s">
         <v>25</v>
       </c>
@@ -3091,7 +3088,7 @@
       <c r="AR32" s="12"/>
       <c r="AS32" s="11"/>
     </row>
-    <row r="33" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:45" ht="16" customHeight="1">
       <c r="D33" t="s">
         <v>26</v>
       </c>
@@ -3138,7 +3135,7 @@
       <c r="AR33" s="12"/>
       <c r="AS33" s="11"/>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:45">
       <c r="D34" t="s">
         <v>27</v>
       </c>
@@ -3185,7 +3182,7 @@
       <c r="AR34" s="12"/>
       <c r="AS34" s="11"/>
     </row>
-    <row r="35" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:45" ht="16" customHeight="1">
       <c r="D35" t="s">
         <v>28</v>
       </c>
@@ -3232,7 +3229,7 @@
       <c r="AR35" s="12"/>
       <c r="AS35" s="11"/>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:45">
       <c r="D36" t="s">
         <v>29</v>
       </c>
@@ -3279,7 +3276,7 @@
       <c r="AR36" s="12"/>
       <c r="AS36" s="11"/>
     </row>
-    <row r="37" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:45" ht="16" customHeight="1">
       <c r="D37" t="s">
         <v>30</v>
       </c>
@@ -3326,7 +3323,7 @@
       <c r="AR37" s="12"/>
       <c r="AS37" s="11"/>
     </row>
-    <row r="38" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:45" ht="16" customHeight="1">
       <c r="D38" t="s">
         <v>31</v>
       </c>
@@ -3373,7 +3370,7 @@
       <c r="AR38" s="12"/>
       <c r="AS38" s="11"/>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:45">
       <c r="D39" t="s">
         <v>32</v>
       </c>
@@ -3420,7 +3417,7 @@
       <c r="AR39" s="12"/>
       <c r="AS39" s="11"/>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:45">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
@@ -3467,7 +3464,7 @@
       <c r="AR40" s="12"/>
       <c r="AS40" s="11"/>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:45">
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
@@ -3568,7 +3565,7 @@
       <c r="AR41" s="12"/>
       <c r="AS41" s="11"/>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:45">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="D42" t="s">
@@ -3617,7 +3614,7 @@
       <c r="AR42" s="12"/>
       <c r="AS42" s="11"/>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:45">
       <c r="D43" t="s">
         <v>18</v>
       </c>
@@ -3664,7 +3661,7 @@
       <c r="AR43" s="12"/>
       <c r="AS43" s="11"/>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:45">
       <c r="D44" t="s">
         <v>19</v>
       </c>
@@ -3711,7 +3708,7 @@
       <c r="AR44" s="12"/>
       <c r="AS44" s="11"/>
     </row>
-    <row r="45" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:45" ht="16" customHeight="1">
       <c r="D45" t="s">
         <v>20</v>
       </c>
@@ -3758,7 +3755,7 @@
       <c r="AR45" s="12"/>
       <c r="AS45" s="11"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:45">
       <c r="D46" t="s">
         <v>21</v>
       </c>
@@ -3805,7 +3802,7 @@
       <c r="AR46" s="12"/>
       <c r="AS46" s="11"/>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:45">
       <c r="D47" t="s">
         <v>22</v>
       </c>
@@ -3852,7 +3849,7 @@
       <c r="AR47" s="12"/>
       <c r="AS47" s="11"/>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:45">
       <c r="D48" t="s">
         <v>23</v>
       </c>
@@ -3899,7 +3896,7 @@
       <c r="AR48" s="12"/>
       <c r="AS48" s="11"/>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:45">
       <c r="D49" t="s">
         <v>24</v>
       </c>
@@ -3946,7 +3943,7 @@
       <c r="AR49" s="12"/>
       <c r="AS49" s="11"/>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:45">
       <c r="D50" t="s">
         <v>25</v>
       </c>
@@ -3993,7 +3990,7 @@
       <c r="AR50" s="12"/>
       <c r="AS50" s="11"/>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:45">
       <c r="D51" t="s">
         <v>26</v>
       </c>
@@ -4024,47 +4021,22 @@
       <c r="AD51" s="20">
         <v>50</v>
       </c>
-      <c r="AE51" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF51" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG51" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH51" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI51" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ51" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK51" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL51" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM51" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN51" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO51" s="29">
-        <v>1</v>
-      </c>
-      <c r="AP51" s="28" t="s">
-        <v>64</v>
-      </c>
+      <c r="AE51" s="21"/>
+      <c r="AG51" s="35"/>
+      <c r="AH51" s="28"/>
+      <c r="AI51" s="36"/>
+      <c r="AJ51" s="37"/>
+      <c r="AK51" s="28"/>
+      <c r="AL51" s="29"/>
+      <c r="AM51" s="38"/>
+      <c r="AN51" s="28"/>
+      <c r="AO51" s="29"/>
+      <c r="AP51" s="28"/>
       <c r="AQ51" s="20"/>
       <c r="AR51" s="20"/>
       <c r="AS51" s="21"/>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:45">
       <c r="D52" t="s">
         <v>27</v>
       </c>
@@ -4093,7 +4065,7 @@
       <c r="AA52" s="10"/>
       <c r="AB52" s="9"/>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:45">
       <c r="D53" t="s">
         <v>28</v>
       </c>
@@ -4127,20 +4099,20 @@
         <v>35</v>
       </c>
       <c r="AI53" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="AK53" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AL53" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM53" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM53" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="AN53" s="31"/>
-    </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.4">
+      <c r="AN53" s="51"/>
+    </row>
+    <row r="54" spans="1:45">
       <c r="D54" t="s">
         <v>29</v>
       </c>
@@ -4178,10 +4150,10 @@
         <v>39</v>
       </c>
       <c r="AL54" s="6"/>
-      <c r="AM54" s="31"/>
-      <c r="AN54" s="31"/>
-    </row>
-    <row r="55" spans="1:45" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AM54" s="51"/>
+      <c r="AN54" s="51"/>
+    </row>
+    <row r="55" spans="1:45" ht="16" customHeight="1">
       <c r="D55" t="s">
         <v>30</v>
       </c>
@@ -4211,22 +4183,20 @@
       <c r="AB55" s="9"/>
       <c r="AE55" s="23"/>
       <c r="AF55" s="23"/>
-      <c r="AH55" s="32" t="s">
+      <c r="AH55" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="AI55" s="35">
-        <v>50</v>
-      </c>
-      <c r="AK55" s="32" t="s">
+      <c r="AI55" s="54"/>
+      <c r="AK55" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="AL55" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM55" s="31"/>
-      <c r="AN55" s="31"/>
-    </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.4">
+      <c r="AL55" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM55" s="51"/>
+      <c r="AN55" s="51"/>
+    </row>
+    <row r="56" spans="1:45">
       <c r="D56" t="s">
         <v>31</v>
       </c>
@@ -4255,12 +4225,12 @@
       <c r="AA56" s="10"/>
       <c r="AB56" s="9"/>
       <c r="AE56" s="10"/>
-      <c r="AH56" s="33"/>
-      <c r="AI56" s="36"/>
-      <c r="AK56" s="34"/>
-      <c r="AL56" s="37"/>
-    </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.4">
+      <c r="AH56" s="52"/>
+      <c r="AI56" s="55"/>
+      <c r="AK56" s="53"/>
+      <c r="AL56" s="56"/>
+    </row>
+    <row r="57" spans="1:45">
       <c r="D57" t="s">
         <v>32</v>
       </c>
@@ -4289,14 +4259,14 @@
       <c r="AA57" s="18"/>
       <c r="AB57" s="19"/>
       <c r="AE57" s="10"/>
-      <c r="AH57" s="34"/>
-      <c r="AI57" s="37"/>
+      <c r="AH57" s="53"/>
+      <c r="AI57" s="56"/>
       <c r="AK57" s="23"/>
       <c r="AL57" s="24"/>
       <c r="AM57" s="23"/>
       <c r="AN57" s="23"/>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:45">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="D58" s="3"/>
@@ -4325,11 +4295,11 @@
       <c r="AA58" s="3"/>
       <c r="AB58" s="3"/>
       <c r="AE58" s="10"/>
-      <c r="AH58" s="32" t="s">
+      <c r="AH58" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="AI58" s="40" t="s">
-        <v>82</v>
+      <c r="AI58" s="47" t="s">
+        <v>74</v>
       </c>
       <c r="AJ58" s="23"/>
       <c r="AK58" s="23"/>
@@ -4337,31 +4307,31 @@
       <c r="AM58" s="23"/>
       <c r="AN58" s="23"/>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:45">
       <c r="AE59" s="10"/>
-      <c r="AH59" s="38"/>
-      <c r="AI59" s="41"/>
+      <c r="AH59" s="45"/>
+      <c r="AI59" s="48"/>
       <c r="AJ59" s="23"/>
       <c r="AK59" s="23"/>
       <c r="AL59" s="24"/>
       <c r="AM59" s="23"/>
       <c r="AN59" s="23"/>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:45">
       <c r="AE60" s="10"/>
-      <c r="AH60" s="39"/>
-      <c r="AI60" s="42"/>
+      <c r="AH60" s="46"/>
+      <c r="AI60" s="49"/>
       <c r="AJ60" s="23"/>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:45">
       <c r="AE61" s="10"/>
       <c r="AJ61" s="23"/>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:45">
       <c r="AE62" s="10"/>
       <c r="AJ62" s="23"/>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:45">
       <c r="AE63" s="10"/>
       <c r="AJ63" s="23"/>
     </row>
@@ -4406,7 +4376,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new way to combine sample and nonsamples list together
</commit_message>
<xml_diff>
--- a/JM1013_worklist_50_Cond_Format.xlsx
+++ b/JM1013_worklist_50_Cond_Format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivint\OneDrive\Desktop\Kelly_Lab\.venv\worklist_git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01c1829094dbd390/Desktop/Kelly_Lab/.venv/worklist_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE238A2-7FF0-4A38-8DF4-507B06B3908E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A45856-9C0F-D140-AD60-2AFFFFA45290}">
   <dimension ref="A1:AV63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="42" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="42" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="AJ63" sqref="AJ63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>